<commit_message>
updated data to include under 25 appearances
</commit_message>
<xml_diff>
--- a/data/blues_appearances.xlsx
+++ b/data/blues_appearances.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\archi\Documents\Javascript Projects\06 Blues Higher or Lower\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\archi\Documents\Javascript Projects\06 Blues Higher or Lower\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00745831-ABFA-4016-95EE-9473A1BDA8CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A4247A-D846-4868-8B86-83FDE9678233}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{467B9E2B-3209-4D33-A819-494DEE8F4CF0}"/>
+    <workbookView xWindow="44280" yWindow="-16290" windowWidth="29040" windowHeight="15840" xr2:uid="{467B9E2B-3209-4D33-A819-494DEE8F4CF0}"/>
   </bookViews>
   <sheets>
     <sheet name="blues_appearances" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="400">
   <si>
     <t>name</t>
   </si>
@@ -621,6 +621,618 @@
   </si>
   <si>
     <t>js</t>
+  </si>
+  <si>
+    <t>Isaac Vassell</t>
+  </si>
+  <si>
+    <t>Darren Anderton</t>
+  </si>
+  <si>
+    <t>Steve Vickers</t>
+  </si>
+  <si>
+    <t>Greg Stewart</t>
+  </si>
+  <si>
+    <t>Will Packwood</t>
+  </si>
+  <si>
+    <t>Chuks Aneke</t>
+  </si>
+  <si>
+    <t>Adam Legzdins</t>
+  </si>
+  <si>
+    <t>Neal Eardley</t>
+  </si>
+  <si>
+    <t>Olly Lee</t>
+  </si>
+  <si>
+    <t>Reece Brown</t>
+  </si>
+  <si>
+    <t>Rowan Vine</t>
+  </si>
+  <si>
+    <t>David Edgar</t>
+  </si>
+  <si>
+    <t>Jesper Grønkjær</t>
+  </si>
+  <si>
+    <t>Fran Villalba</t>
+  </si>
+  <si>
+    <t>Alen Halilović</t>
+  </si>
+  <si>
+    <t>James Vaughan</t>
+  </si>
+  <si>
+    <t>Sam Cosgrove</t>
+  </si>
+  <si>
+    <t>Trésor Luntala</t>
+  </si>
+  <si>
+    <t>Nico Gordon</t>
+  </si>
+  <si>
+    <t>Adam Clayton</t>
+  </si>
+  <si>
+    <t>Dwight Yorke</t>
+  </si>
+  <si>
+    <t>Koby Arthur</t>
+  </si>
+  <si>
+    <t>Martin Jiránek</t>
+  </si>
+  <si>
+    <t>Charlie Lakin</t>
+  </si>
+  <si>
+    <t>Connal Trueman</t>
+  </si>
+  <si>
+    <t>Darryl Powell</t>
+  </si>
+  <si>
+    <t>Kerim Frei</t>
+  </si>
+  <si>
+    <t>Robbie Blake</t>
+  </si>
+  <si>
+    <t>Steve Seddon</t>
+  </si>
+  <si>
+    <t>Daniël de Ridder</t>
+  </si>
+  <si>
+    <t>Matt Green</t>
+  </si>
+  <si>
+    <t>Míchel</t>
+  </si>
+  <si>
+    <t>Alex Bruce</t>
+  </si>
+  <si>
+    <t>Cheick Keita</t>
+  </si>
+  <si>
+    <t>Chris Sutton</t>
+  </si>
+  <si>
+    <t>Jason Lowe</t>
+  </si>
+  <si>
+    <t>Marcos Painter</t>
+  </si>
+  <si>
+    <t>Josh McEachran</t>
+  </si>
+  <si>
+    <t>Darren Ambrose</t>
+  </si>
+  <si>
+    <t>Alex Pritchard</t>
+  </si>
+  <si>
+    <t>Grégory Vignal</t>
+  </si>
+  <si>
+    <t>Caolan Boyd-Munce</t>
+  </si>
+  <si>
+    <t>Eddie Newton</t>
+  </si>
+  <si>
+    <t>Aaron Martin</t>
+  </si>
+  <si>
+    <t>Nicolai Brock-Madsen</t>
+  </si>
+  <si>
+    <t>Odin Bailey</t>
+  </si>
+  <si>
+    <t>Marcel Oakley</t>
+  </si>
+  <si>
+    <t>Joey Hutchinson</t>
+  </si>
+  <si>
+    <t>Mark Duffy</t>
+  </si>
+  <si>
+    <t>Brian Howard</t>
+  </si>
+  <si>
+    <t>Amari Miller</t>
+  </si>
+  <si>
+    <t>Jack Storer</t>
+  </si>
+  <si>
+    <t>Bez Lubala</t>
+  </si>
+  <si>
+    <t>Jake Jervis</t>
+  </si>
+  <si>
+    <t>Tom Williams</t>
+  </si>
+  <si>
+    <t>Zach Jeacock</t>
+  </si>
+  <si>
+    <t>Jayden Reid</t>
+  </si>
+  <si>
+    <t>Jacques Williams</t>
+  </si>
+  <si>
+    <t>Ryan Stirk</t>
+  </si>
+  <si>
+    <t>Craig Fagan</t>
+  </si>
+  <si>
+    <t>Tate Campbell</t>
+  </si>
+  <si>
+    <t>Guy Moussi</t>
+  </si>
+  <si>
+    <t>Charlee Adams</t>
+  </si>
+  <si>
+    <t>Geraldo Bajrami</t>
+  </si>
+  <si>
+    <t>Mathew Birley</t>
+  </si>
+  <si>
+    <t>Richard Kingson</t>
+  </si>
+  <si>
+    <t>Jay O'Shea</t>
+  </si>
+  <si>
+    <t>Papa Bouba Diop</t>
+  </si>
+  <si>
+    <t>Dariusz Dudka</t>
+  </si>
+  <si>
+    <t>Denny Johnstone</t>
+  </si>
+  <si>
+    <t>Luciano Figueroa</t>
+  </si>
+  <si>
+    <t>Shane Lowry</t>
+  </si>
+  <si>
+    <t>Agus Medina</t>
+  </si>
+  <si>
+    <t>Adan George</t>
+  </si>
+  <si>
+    <t>Keyendrah Simmonds</t>
+  </si>
+  <si>
+    <t>Mitch Roberts</t>
+  </si>
+  <si>
+    <t>Giovanny Espinoza</t>
+  </si>
+  <si>
+    <t>Enric Vallès</t>
+  </si>
+  <si>
+    <t>Andrés Prieto</t>
+  </si>
+  <si>
+    <t>Andy Marriott</t>
+  </si>
+  <si>
+    <t>Andrew Barrowman</t>
+  </si>
+  <si>
+    <t>Jared Wilson</t>
+  </si>
+  <si>
+    <t>Ulises de la Cruz</t>
+  </si>
+  <si>
+    <t>Amari'i Bell</t>
+  </si>
+  <si>
+    <t>Corey O'Keeffe</t>
+  </si>
+  <si>
+    <t>Ryan Burke</t>
+  </si>
+  <si>
+    <t>Miguel Fernández</t>
+  </si>
+  <si>
+    <t>Peter Till</t>
+  </si>
+  <si>
+    <t>Sam Oji</t>
+  </si>
+  <si>
+    <t>Sone Aluko</t>
+  </si>
+  <si>
+    <t>Robin Shroot</t>
+  </si>
+  <si>
+    <t>Dan Preston</t>
+  </si>
+  <si>
+    <t>Ashley Sammons</t>
+  </si>
+  <si>
+    <t>Akwasi Asante</t>
+  </si>
+  <si>
+    <t>Eddy Gnahoré</t>
+  </si>
+  <si>
+    <t>David Lucas</t>
+  </si>
+  <si>
+    <t>Reece Hales</t>
+  </si>
+  <si>
+    <t>Gavin Gunning</t>
+  </si>
+  <si>
+    <t>Dan Scarr</t>
+  </si>
+  <si>
+    <t>Jack Concannon</t>
+  </si>
+  <si>
+    <t>Alexander Hleb</t>
+  </si>
+  <si>
+    <t>Matija Sarkic</t>
+  </si>
+  <si>
+    <t>Oliver Burke</t>
+  </si>
+  <si>
+    <t>Onel Hernández</t>
+  </si>
+  <si>
+    <t>Quincy Owusu-Abeyie</t>
+  </si>
+  <si>
+    <t>Tyler Roberts</t>
+  </si>
+  <si>
+    <t>Kemy Agustien</t>
+  </si>
+  <si>
+    <t>Matt Derbyshire</t>
+  </si>
+  <si>
+    <t>Alfie Chang</t>
+  </si>
+  <si>
+    <t>Lloyd Dyer</t>
+  </si>
+  <si>
+    <t>Kyle Bartley</t>
+  </si>
+  <si>
+    <t>Federico Macheda</t>
+  </si>
+  <si>
+    <t>Rekeem Harper</t>
+  </si>
+  <si>
+    <t>Jefferson Montero</t>
+  </si>
+  <si>
+    <t>Emyr Huws</t>
+  </si>
+  <si>
+    <t>Mark Burchill</t>
+  </si>
+  <si>
+    <t>Hamer Bouazza</t>
+  </si>
+  <si>
+    <t>Rafael Schmitz</t>
+  </si>
+  <si>
+    <t>Andros Townsend</t>
+  </si>
+  <si>
+    <t>Omar Bogle</t>
+  </si>
+  <si>
+    <t>Peter Ramage</t>
+  </si>
+  <si>
+    <t>Reda Khadra</t>
+  </si>
+  <si>
+    <t>David Bentley</t>
+  </si>
+  <si>
+    <t>Mauro Zárate</t>
+  </si>
+  <si>
+    <t>Scott Sinclair</t>
+  </si>
+  <si>
+    <t>Lyle Taylor</t>
+  </si>
+  <si>
+    <t>Isaiah Rankin</t>
+  </si>
+  <si>
+    <t>Johan Djourou</t>
+  </si>
+  <si>
+    <t>Rob Hall</t>
+  </si>
+  <si>
+    <t>Jesse Lingard</t>
+  </si>
+  <si>
+    <t>Rob Kiernan</t>
+  </si>
+  <si>
+    <t>Peter Atherton</t>
+  </si>
+  <si>
+    <t>Alex Cochrane</t>
+  </si>
+  <si>
+    <t>Alfie May</t>
+  </si>
+  <si>
+    <t>Emil Hansson</t>
+  </si>
+  <si>
+    <t>Nicky Hunt</t>
+  </si>
+  <si>
+    <t>Erik Huseklepp</t>
+  </si>
+  <si>
+    <t>Jordon Ibe</t>
+  </si>
+  <si>
+    <t>Nigel Quashie</t>
+  </si>
+  <si>
+    <t>Christoph Klarer</t>
+  </si>
+  <si>
+    <t>Leroy Lita</t>
+  </si>
+  <si>
+    <t>Will Buckley</t>
+  </si>
+  <si>
+    <t>Andre Dozzell</t>
+  </si>
+  <si>
+    <t>Teden Mengi</t>
+  </si>
+  <si>
+    <t>Willum Þór Willumsson</t>
+  </si>
+  <si>
+    <t>Romelle Donovan</t>
+  </si>
+  <si>
+    <t>Marc Leonard</t>
+  </si>
+  <si>
+    <t>Thomas Myhre</t>
+  </si>
+  <si>
+    <t>Grant Hall</t>
+  </si>
+  <si>
+    <t>Carl Jenkinson</t>
+  </si>
+  <si>
+    <t>Alfons Sampsted</t>
+  </si>
+  <si>
+    <t>Josh Williams</t>
+  </si>
+  <si>
+    <t>Carlos Costly</t>
+  </si>
+  <si>
+    <t>Tyler Blackett</t>
+  </si>
+  <si>
+    <t>Wilson Palacios</t>
+  </si>
+  <si>
+    <t>Taylor Gardner-Hickman</t>
+  </si>
+  <si>
+    <t>Cohen Bramall</t>
+  </si>
+  <si>
+    <t>Aaron McLean</t>
+  </si>
+  <si>
+    <t>Yan Valery</t>
+  </si>
+  <si>
+    <t>Bailey Peacock-Farrell</t>
+  </si>
+  <si>
+    <t>Martin Latka</t>
+  </si>
+  <si>
+    <t>Scott Allan</t>
+  </si>
+  <si>
+    <t>Curtis Fleming</t>
+  </si>
+  <si>
+    <t>Alan Kelly</t>
+  </si>
+  <si>
+    <t>Teemu Tainio</t>
+  </si>
+  <si>
+    <t>Tom Thorpe</t>
+  </si>
+  <si>
+    <t>Brek Shea</t>
+  </si>
+  <si>
+    <t>Kyle Lafferty</t>
+  </si>
+  <si>
+    <t>Taylor Richards</t>
+  </si>
+  <si>
+    <t>Lyndon Dykes</t>
+  </si>
+  <si>
+    <t>Tomoki Iwata</t>
+  </si>
+  <si>
+    <t>Scott Wright</t>
+  </si>
+  <si>
+    <t>Obafemi Martins</t>
+  </si>
+  <si>
+    <t>Brandon Khela</t>
+  </si>
+  <si>
+    <t>Jamie Pollock</t>
+  </si>
+  <si>
+    <t>Andy Cole</t>
+  </si>
+  <si>
+    <t>Jerome Sinclair</t>
+  </si>
+  <si>
+    <t>Przemysław Płacheta</t>
+  </si>
+  <si>
+    <t>Arkadiusz Bąk</t>
+  </si>
+  <si>
+    <t>Luke Harris</t>
+  </si>
+  <si>
+    <t>Juan Castillo</t>
+  </si>
+  <si>
+    <t>Ayumu Yokoyama</t>
+  </si>
+  <si>
+    <t>Ryan Allsop</t>
+  </si>
+  <si>
+    <t>Carlos Ferrari</t>
+  </si>
+  <si>
+    <t>Steve Jenkins</t>
+  </si>
+  <si>
+    <t>Albert Rusnák</t>
+  </si>
+  <si>
+    <t>Ben Davies</t>
+  </si>
+  <si>
+    <t>Richard Edghill</t>
+  </si>
+  <si>
+    <t>Gary Charles</t>
+  </si>
+  <si>
+    <t>Bjørn Otto Bragstad</t>
+  </si>
+  <si>
+    <t>Michael Hughes</t>
+  </si>
+  <si>
+    <t>Djimi Traoré</t>
+  </si>
+  <si>
+    <t>James Hurst</t>
+  </si>
+  <si>
+    <t>Greg Halford</t>
+  </si>
+  <si>
+    <t>Liam Walsh</t>
+  </si>
+  <si>
+    <t>Michael Carrick</t>
+  </si>
+  <si>
+    <t>Stuart Campbell</t>
+  </si>
+  <si>
+    <t>Salif Diao</t>
+  </si>
+  <si>
+    <t>Borja Oubiña</t>
+  </si>
+  <si>
+    <t>Rhoys Wiggins</t>
+  </si>
+  <si>
+    <t>Ferdinand Coly</t>
+  </si>
+  <si>
+    <t>Ben Gordon</t>
+  </si>
+  <si>
+    <t>Carl Tiler</t>
+  </si>
+  <si>
+    <t>Piotr Świerczewski</t>
   </si>
 </sst>
 </file>
@@ -1481,10 +2093,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EEF3C80-EC9D-49C8-BAAC-C0F8602D5396}">
-  <dimension ref="A1:E192"/>
+  <dimension ref="A1:E396"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E192"/>
+    <sheetView tabSelected="1" topLeftCell="A360" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E396"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3848,7 +4460,7 @@
         <v>0</v>
       </c>
       <c r="E131" t="str">
-        <f t="shared" ref="E131:E192" si="2">"{ name: '" &amp; A131 &amp; "', appearances: " &amp; C131 &amp; " },"</f>
+        <f t="shared" ref="E131:E194" si="2">"{ name: '" &amp; A131 &amp; "', appearances: " &amp; C131 &amp; " },"</f>
         <v>{ name: 'Jack Butland', appearances: 46 },</v>
       </c>
     </row>
@@ -4946,8 +5558,3680 @@
         <v>0</v>
       </c>
       <c r="E192" t="str">
-        <f>"{ name: '" &amp; A192 &amp; "', appearances: " &amp; C192 &amp; " }"</f>
-        <v>{ name: 'Emanuel Aiwu', appearances: 25 }</v>
+        <f t="shared" si="2"/>
+        <v>{ name: 'Emanuel Aiwu', appearances: 25 },</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A193" t="s">
+        <v>196</v>
+      </c>
+      <c r="B193">
+        <v>2019</v>
+      </c>
+      <c r="C193">
+        <v>24</v>
+      </c>
+      <c r="D193">
+        <v>1</v>
+      </c>
+      <c r="E193" t="str">
+        <f t="shared" si="2"/>
+        <v>{ name: 'Isaac Vassell', appearances: 24 },</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A194" t="s">
+        <v>197</v>
+      </c>
+      <c r="B194">
+        <v>2005</v>
+      </c>
+      <c r="C194">
+        <v>24</v>
+      </c>
+      <c r="D194">
+        <v>3</v>
+      </c>
+      <c r="E194" t="str">
+        <f t="shared" si="2"/>
+        <v>{ name: 'Darren Anderton', appearances: 24 },</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A195" t="s">
+        <v>296</v>
+      </c>
+      <c r="B195">
+        <v>2011</v>
+      </c>
+      <c r="C195">
+        <v>24</v>
+      </c>
+      <c r="D195">
+        <v>2</v>
+      </c>
+      <c r="E195" t="str">
+        <f t="shared" ref="E195:E258" si="3">"{ name: '" &amp; A195 &amp; "', appearances: " &amp; C195 &amp; " },"</f>
+        <v>{ name: 'Alexander Hleb', appearances: 24 },</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A196" t="s">
+        <v>297</v>
+      </c>
+      <c r="B196">
+        <v>2022</v>
+      </c>
+      <c r="C196">
+        <v>23</v>
+      </c>
+      <c r="D196">
+        <v>0</v>
+      </c>
+      <c r="E196" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Matija Sarkic', appearances: 23 },</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A197" t="s">
+        <v>298</v>
+      </c>
+      <c r="B197">
+        <v>2024</v>
+      </c>
+      <c r="C197">
+        <v>23</v>
+      </c>
+      <c r="D197">
+        <v>0</v>
+      </c>
+      <c r="E197" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Oliver Burke', appearances: 23 },</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A198" t="s">
+        <v>198</v>
+      </c>
+      <c r="B198">
+        <v>2003</v>
+      </c>
+      <c r="C198">
+        <v>23</v>
+      </c>
+      <c r="D198">
+        <v>1</v>
+      </c>
+      <c r="E198" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Steve Vickers', appearances: 23 },</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A199" t="s">
+        <v>299</v>
+      </c>
+      <c r="B199">
+        <v>2022</v>
+      </c>
+      <c r="C199">
+        <v>22</v>
+      </c>
+      <c r="D199">
+        <v>3</v>
+      </c>
+      <c r="E199" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Onel Hernández', appearances: 22 },</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A200" t="s">
+        <v>199</v>
+      </c>
+      <c r="B200">
+        <v>2017</v>
+      </c>
+      <c r="C200">
+        <v>22</v>
+      </c>
+      <c r="D200">
+        <v>0</v>
+      </c>
+      <c r="E200" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Greg Stewart', appearances: 22 },</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A201" t="s">
+        <v>300</v>
+      </c>
+      <c r="B201">
+        <v>2008</v>
+      </c>
+      <c r="C201">
+        <v>21</v>
+      </c>
+      <c r="D201">
+        <v>3</v>
+      </c>
+      <c r="E201" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Quincy Owusu-Abeyie', appearances: 21 },</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A202" t="s">
+        <v>200</v>
+      </c>
+      <c r="B202">
+        <v>2014</v>
+      </c>
+      <c r="C202">
+        <v>21</v>
+      </c>
+      <c r="D202">
+        <v>0</v>
+      </c>
+      <c r="E202" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Will Packwood', appearances: 21 },</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A203" t="s">
+        <v>201</v>
+      </c>
+      <c r="B203">
+        <v>2022</v>
+      </c>
+      <c r="C203">
+        <v>21</v>
+      </c>
+      <c r="D203">
+        <v>2</v>
+      </c>
+      <c r="E203" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Chuks Aneke', appearances: 21 },</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A204" t="s">
+        <v>301</v>
+      </c>
+      <c r="B204">
+        <v>2023</v>
+      </c>
+      <c r="C204">
+        <v>21</v>
+      </c>
+      <c r="D204">
+        <v>0</v>
+      </c>
+      <c r="E204" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Tyler Roberts', appearances: 21 },</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A205" t="s">
+        <v>202</v>
+      </c>
+      <c r="B205">
+        <v>2017</v>
+      </c>
+      <c r="C205">
+        <v>21</v>
+      </c>
+      <c r="D205">
+        <v>0</v>
+      </c>
+      <c r="E205" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Adam Legzdins', appearances: 21 },</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A206" t="s">
+        <v>203</v>
+      </c>
+      <c r="B206">
+        <v>2016</v>
+      </c>
+      <c r="C206">
+        <v>21</v>
+      </c>
+      <c r="D206">
+        <v>0</v>
+      </c>
+      <c r="E206" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Neal Eardley', appearances: 21 },</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A207" t="s">
+        <v>302</v>
+      </c>
+      <c r="B207">
+        <v>2009</v>
+      </c>
+      <c r="C207">
+        <v>20</v>
+      </c>
+      <c r="D207">
+        <v>0</v>
+      </c>
+      <c r="E207" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Kemy Agustien', appearances: 20 },</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A208" t="s">
+        <v>204</v>
+      </c>
+      <c r="B208">
+        <v>2014</v>
+      </c>
+      <c r="C208">
+        <v>20</v>
+      </c>
+      <c r="D208">
+        <v>2</v>
+      </c>
+      <c r="E208" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Olly Lee', appearances: 20 },</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A209" t="s">
+        <v>205</v>
+      </c>
+      <c r="B209">
+        <v>2017</v>
+      </c>
+      <c r="C209">
+        <v>20</v>
+      </c>
+      <c r="D209">
+        <v>0</v>
+      </c>
+      <c r="E209" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Reece Brown', appearances: 20 },</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A210" t="s">
+        <v>303</v>
+      </c>
+      <c r="B210">
+        <v>2011</v>
+      </c>
+      <c r="C210">
+        <v>20</v>
+      </c>
+      <c r="D210">
+        <v>3</v>
+      </c>
+      <c r="E210" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Matt Derbyshire', appearances: 20 },</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A211" t="s">
+        <v>304</v>
+      </c>
+      <c r="B211">
+        <v>2021</v>
+      </c>
+      <c r="C211">
+        <v>20</v>
+      </c>
+      <c r="D211">
+        <v>0</v>
+      </c>
+      <c r="E211" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Alfie Chang', appearances: 20 },</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A212" t="s">
+        <v>305</v>
+      </c>
+      <c r="B212">
+        <v>2015</v>
+      </c>
+      <c r="C212">
+        <v>19</v>
+      </c>
+      <c r="D212">
+        <v>1</v>
+      </c>
+      <c r="E212" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Lloyd Dyer', appearances: 19 },</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A213" t="s">
+        <v>206</v>
+      </c>
+      <c r="B213">
+        <v>2007</v>
+      </c>
+      <c r="C213">
+        <v>19</v>
+      </c>
+      <c r="D213">
+        <v>1</v>
+      </c>
+      <c r="E213" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Rowan Vine', appearances: 19 },</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A214" t="s">
+        <v>306</v>
+      </c>
+      <c r="B214">
+        <v>2014</v>
+      </c>
+      <c r="C214">
+        <v>19</v>
+      </c>
+      <c r="D214">
+        <v>5</v>
+      </c>
+      <c r="E214" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Kyle Bartley', appearances: 19 },</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A215" t="s">
+        <v>207</v>
+      </c>
+      <c r="B215">
+        <v>2015</v>
+      </c>
+      <c r="C215">
+        <v>19</v>
+      </c>
+      <c r="D215">
+        <v>1</v>
+      </c>
+      <c r="E215" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'David Edgar', appearances: 19 },</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A216" t="s">
+        <v>307</v>
+      </c>
+      <c r="B216">
+        <v>2014</v>
+      </c>
+      <c r="C216">
+        <v>18</v>
+      </c>
+      <c r="D216">
+        <v>10</v>
+      </c>
+      <c r="E216" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Federico Macheda', appearances: 18 },</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A217" t="s">
+        <v>308</v>
+      </c>
+      <c r="B217">
+        <v>2021</v>
+      </c>
+      <c r="C217">
+        <v>18</v>
+      </c>
+      <c r="D217">
+        <v>0</v>
+      </c>
+      <c r="E217" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Rekeem Harper', appearances: 18 },</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A218" t="s">
+        <v>208</v>
+      </c>
+      <c r="B218">
+        <v>2004</v>
+      </c>
+      <c r="C218">
+        <v>18</v>
+      </c>
+      <c r="D218">
+        <v>1</v>
+      </c>
+      <c r="E218" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Jesper Grønkjær', appearances: 18 },</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A219" t="s">
+        <v>309</v>
+      </c>
+      <c r="B219">
+        <v>2020</v>
+      </c>
+      <c r="C219">
+        <v>18</v>
+      </c>
+      <c r="D219">
+        <v>0</v>
+      </c>
+      <c r="E219" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Jefferson Montero', appearances: 18 },</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A220" t="s">
+        <v>310</v>
+      </c>
+      <c r="B220">
+        <v>2014</v>
+      </c>
+      <c r="C220">
+        <v>17</v>
+      </c>
+      <c r="D220">
+        <v>2</v>
+      </c>
+      <c r="E220" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Emyr Huws', appearances: 17 },</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A221" t="s">
+        <v>209</v>
+      </c>
+      <c r="B221">
+        <v>2019</v>
+      </c>
+      <c r="C221">
+        <v>17</v>
+      </c>
+      <c r="D221">
+        <v>1</v>
+      </c>
+      <c r="E221" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Fran Villalba', appearances: 17 },</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A222" t="s">
+        <v>210</v>
+      </c>
+      <c r="B222">
+        <v>2021</v>
+      </c>
+      <c r="C222">
+        <v>17</v>
+      </c>
+      <c r="D222">
+        <v>1</v>
+      </c>
+      <c r="E222" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Alen Halilović', appearances: 17 },</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A223" t="s">
+        <v>211</v>
+      </c>
+      <c r="B223">
+        <v>2016</v>
+      </c>
+      <c r="C223">
+        <v>17</v>
+      </c>
+      <c r="D223">
+        <v>0</v>
+      </c>
+      <c r="E223" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'James Vaughan', appearances: 17 },</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A224" t="s">
+        <v>212</v>
+      </c>
+      <c r="B224">
+        <v>2023</v>
+      </c>
+      <c r="C224">
+        <v>17</v>
+      </c>
+      <c r="D224">
+        <v>0</v>
+      </c>
+      <c r="E224" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Sam Cosgrove', appearances: 17 },</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A225" t="s">
+        <v>311</v>
+      </c>
+      <c r="B225">
+        <v>2000</v>
+      </c>
+      <c r="C225">
+        <v>17</v>
+      </c>
+      <c r="D225">
+        <v>5</v>
+      </c>
+      <c r="E225" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Mark Burchill', appearances: 17 },</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A226" t="s">
+        <v>312</v>
+      </c>
+      <c r="B226">
+        <v>2009</v>
+      </c>
+      <c r="C226">
+        <v>16</v>
+      </c>
+      <c r="D226">
+        <v>1</v>
+      </c>
+      <c r="E226" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Hamer Bouazza', appearances: 16 },</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A227" t="s">
+        <v>213</v>
+      </c>
+      <c r="B227">
+        <v>2001</v>
+      </c>
+      <c r="C227">
+        <v>16</v>
+      </c>
+      <c r="D227">
+        <v>0</v>
+      </c>
+      <c r="E227" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Trésor Luntala', appearances: 16 },</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A228" t="s">
+        <v>313</v>
+      </c>
+      <c r="B228">
+        <v>2008</v>
+      </c>
+      <c r="C228">
+        <v>16</v>
+      </c>
+      <c r="D228">
+        <v>0</v>
+      </c>
+      <c r="E228" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Rafael Schmitz', appearances: 16 },</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A229" t="s">
+        <v>314</v>
+      </c>
+      <c r="B229">
+        <v>2012</v>
+      </c>
+      <c r="C229">
+        <v>16</v>
+      </c>
+      <c r="D229">
+        <v>0</v>
+      </c>
+      <c r="E229" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Andros Townsend', appearances: 16 },</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A230" t="s">
+        <v>315</v>
+      </c>
+      <c r="B230">
+        <v>2018</v>
+      </c>
+      <c r="C230">
+        <v>16</v>
+      </c>
+      <c r="D230">
+        <v>1</v>
+      </c>
+      <c r="E230" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Omar Bogle', appearances: 16 },</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A231" t="s">
+        <v>214</v>
+      </c>
+      <c r="B231">
+        <v>2022</v>
+      </c>
+      <c r="C231">
+        <v>16</v>
+      </c>
+      <c r="D231">
+        <v>1</v>
+      </c>
+      <c r="E231" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Nico Gordon', appearances: 16 },</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A232" t="s">
+        <v>316</v>
+      </c>
+      <c r="B232">
+        <v>2012</v>
+      </c>
+      <c r="C232">
+        <v>16</v>
+      </c>
+      <c r="D232">
+        <v>0</v>
+      </c>
+      <c r="E232" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Peter Ramage', appearances: 16 },</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A233" t="s">
+        <v>215</v>
+      </c>
+      <c r="B233">
+        <v>2021</v>
+      </c>
+      <c r="C233">
+        <v>16</v>
+      </c>
+      <c r="D233">
+        <v>0</v>
+      </c>
+      <c r="E233" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Adam Clayton', appearances: 16 },</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A234" t="s">
+        <v>317</v>
+      </c>
+      <c r="B234">
+        <v>2023</v>
+      </c>
+      <c r="C234">
+        <v>16</v>
+      </c>
+      <c r="D234">
+        <v>4</v>
+      </c>
+      <c r="E234" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Reda Khadra', appearances: 16 },</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A235" t="s">
+        <v>216</v>
+      </c>
+      <c r="B235">
+        <v>2005</v>
+      </c>
+      <c r="C235">
+        <v>16</v>
+      </c>
+      <c r="D235">
+        <v>2</v>
+      </c>
+      <c r="E235" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Dwight Yorke', appearances: 16 },</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A236" t="s">
+        <v>217</v>
+      </c>
+      <c r="B236">
+        <v>2015</v>
+      </c>
+      <c r="C236">
+        <v>16</v>
+      </c>
+      <c r="D236">
+        <v>0</v>
+      </c>
+      <c r="E236" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Koby Arthur', appearances: 16 },</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A237" t="s">
+        <v>218</v>
+      </c>
+      <c r="B237">
+        <v>2011</v>
+      </c>
+      <c r="C237">
+        <v>16</v>
+      </c>
+      <c r="D237">
+        <v>0</v>
+      </c>
+      <c r="E237" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Martin Jiránek', appearances: 16 },</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A238" t="s">
+        <v>219</v>
+      </c>
+      <c r="B238">
+        <v>2021</v>
+      </c>
+      <c r="C238">
+        <v>16</v>
+      </c>
+      <c r="D238">
+        <v>0</v>
+      </c>
+      <c r="E238" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Charlie Lakin', appearances: 16 },</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A239" t="s">
+        <v>220</v>
+      </c>
+      <c r="B239">
+        <v>2022</v>
+      </c>
+      <c r="C239">
+        <v>15</v>
+      </c>
+      <c r="D239">
+        <v>0</v>
+      </c>
+      <c r="E239" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Connal Trueman', appearances: 15 },</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A240" t="s">
+        <v>318</v>
+      </c>
+      <c r="B240">
+        <v>2011</v>
+      </c>
+      <c r="C240">
+        <v>15</v>
+      </c>
+      <c r="D240">
+        <v>1</v>
+      </c>
+      <c r="E240" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'David Bentley', appearances: 15 },</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A241" t="s">
+        <v>319</v>
+      </c>
+      <c r="B241">
+        <v>2008</v>
+      </c>
+      <c r="C241">
+        <v>14</v>
+      </c>
+      <c r="D241">
+        <v>4</v>
+      </c>
+      <c r="E241" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Mauro Zárate', appearances: 14 },</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A242" t="s">
+        <v>320</v>
+      </c>
+      <c r="B242">
+        <v>2009</v>
+      </c>
+      <c r="C242">
+        <v>14</v>
+      </c>
+      <c r="D242">
+        <v>0</v>
+      </c>
+      <c r="E242" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Scott Sinclair', appearances: 14 },</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A243" t="s">
+        <v>321</v>
+      </c>
+      <c r="B243">
+        <v>2022</v>
+      </c>
+      <c r="C243">
+        <v>14</v>
+      </c>
+      <c r="D243">
+        <v>5</v>
+      </c>
+      <c r="E243" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Lyle Taylor', appearances: 14 },</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A244" t="s">
+        <v>221</v>
+      </c>
+      <c r="B244">
+        <v>2003</v>
+      </c>
+      <c r="C244">
+        <v>14</v>
+      </c>
+      <c r="D244">
+        <v>0</v>
+      </c>
+      <c r="E244" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Darryl Powell', appearances: 14 },</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A245" t="s">
+        <v>322</v>
+      </c>
+      <c r="B245">
+        <v>2000</v>
+      </c>
+      <c r="C245">
+        <v>13</v>
+      </c>
+      <c r="D245">
+        <v>4</v>
+      </c>
+      <c r="E245" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Isaiah Rankin', appearances: 13 },</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A246" t="s">
+        <v>323</v>
+      </c>
+      <c r="B246">
+        <v>2007</v>
+      </c>
+      <c r="C246">
+        <v>13</v>
+      </c>
+      <c r="D246">
+        <v>0</v>
+      </c>
+      <c r="E246" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Johan Djourou', appearances: 13 },</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A247" t="s">
+        <v>324</v>
+      </c>
+      <c r="B247">
+        <v>2013</v>
+      </c>
+      <c r="C247">
+        <v>13</v>
+      </c>
+      <c r="D247">
+        <v>0</v>
+      </c>
+      <c r="E247" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Rob Hall', appearances: 13 },</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A248" t="s">
+        <v>325</v>
+      </c>
+      <c r="B248">
+        <v>2013</v>
+      </c>
+      <c r="C248">
+        <v>13</v>
+      </c>
+      <c r="D248">
+        <v>6</v>
+      </c>
+      <c r="E248" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Jesse Lingard', appearances: 13 },</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A249" t="s">
+        <v>222</v>
+      </c>
+      <c r="B249">
+        <v>2017</v>
+      </c>
+      <c r="C249">
+        <v>13</v>
+      </c>
+      <c r="D249">
+        <v>1</v>
+      </c>
+      <c r="E249" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Kerim Frei', appearances: 13 },</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A250" t="s">
+        <v>223</v>
+      </c>
+      <c r="B250">
+        <v>2005</v>
+      </c>
+      <c r="C250">
+        <v>13</v>
+      </c>
+      <c r="D250">
+        <v>2</v>
+      </c>
+      <c r="E250" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Robbie Blake', appearances: 13 },</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A251" t="s">
+        <v>326</v>
+      </c>
+      <c r="B251">
+        <v>2015</v>
+      </c>
+      <c r="C251">
+        <v>12</v>
+      </c>
+      <c r="D251">
+        <v>1</v>
+      </c>
+      <c r="E251" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Rob Kiernan', appearances: 12 },</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A252" t="s">
+        <v>224</v>
+      </c>
+      <c r="B252">
+        <v>2021</v>
+      </c>
+      <c r="C252">
+        <v>12</v>
+      </c>
+      <c r="D252">
+        <v>0</v>
+      </c>
+      <c r="E252" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Steve Seddon', appearances: 12 },</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A253" t="s">
+        <v>327</v>
+      </c>
+      <c r="B253">
+        <v>2001</v>
+      </c>
+      <c r="C253">
+        <v>12</v>
+      </c>
+      <c r="D253">
+        <v>0</v>
+      </c>
+      <c r="E253" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Peter Atherton', appearances: 12 },</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A254" t="s">
+        <v>225</v>
+      </c>
+      <c r="B254">
+        <v>2008</v>
+      </c>
+      <c r="C254">
+        <v>12</v>
+      </c>
+      <c r="D254">
+        <v>0</v>
+      </c>
+      <c r="E254" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Daniël de Ridder', appearances: 12 },</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A255" t="s">
+        <v>226</v>
+      </c>
+      <c r="B255">
+        <v>2013</v>
+      </c>
+      <c r="C255">
+        <v>12</v>
+      </c>
+      <c r="D255">
+        <v>2</v>
+      </c>
+      <c r="E255" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Matt Green', appearances: 12 },</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A256" t="s">
+        <v>227</v>
+      </c>
+      <c r="B256">
+        <v>2010</v>
+      </c>
+      <c r="C256">
+        <v>12</v>
+      </c>
+      <c r="D256">
+        <v>0</v>
+      </c>
+      <c r="E256" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Míchel', appearances: 12 },</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A257" t="s">
+        <v>328</v>
+      </c>
+      <c r="B257">
+        <v>2024</v>
+      </c>
+      <c r="C257">
+        <v>12</v>
+      </c>
+      <c r="D257">
+        <v>0</v>
+      </c>
+      <c r="E257" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Alex Cochrane', appearances: 12 },</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A258" t="s">
+        <v>329</v>
+      </c>
+      <c r="B258">
+        <v>2024</v>
+      </c>
+      <c r="C258">
+        <v>12</v>
+      </c>
+      <c r="D258">
+        <v>5</v>
+      </c>
+      <c r="E258" t="str">
+        <f t="shared" si="3"/>
+        <v>{ name: 'Alfie May', appearances: 12 },</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A259" t="s">
+        <v>330</v>
+      </c>
+      <c r="B259">
+        <v>2024</v>
+      </c>
+      <c r="C259">
+        <v>12</v>
+      </c>
+      <c r="D259">
+        <v>0</v>
+      </c>
+      <c r="E259" t="str">
+        <f t="shared" ref="E259:E322" si="4">"{ name: '" &amp; A259 &amp; "', appearances: " &amp; C259 &amp; " },"</f>
+        <v>{ name: 'Emil Hansson', appearances: 12 },</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A260" t="s">
+        <v>228</v>
+      </c>
+      <c r="B260">
+        <v>2006</v>
+      </c>
+      <c r="C260">
+        <v>12</v>
+      </c>
+      <c r="D260">
+        <v>0</v>
+      </c>
+      <c r="E260" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Alex Bruce', appearances: 12 },</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A261" t="s">
+        <v>331</v>
+      </c>
+      <c r="B261">
+        <v>2008</v>
+      </c>
+      <c r="C261">
+        <v>11</v>
+      </c>
+      <c r="D261">
+        <v>0</v>
+      </c>
+      <c r="E261" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Nicky Hunt', appearances: 11 },</v>
+      </c>
+    </row>
+    <row r="262" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A262" t="s">
+        <v>332</v>
+      </c>
+      <c r="B262">
+        <v>2012</v>
+      </c>
+      <c r="C262">
+        <v>11</v>
+      </c>
+      <c r="D262">
+        <v>2</v>
+      </c>
+      <c r="E262" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Erik Huseklepp', appearances: 11 },</v>
+      </c>
+    </row>
+    <row r="263" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A263" t="s">
+        <v>333</v>
+      </c>
+      <c r="B263">
+        <v>2014</v>
+      </c>
+      <c r="C263">
+        <v>11</v>
+      </c>
+      <c r="D263">
+        <v>1</v>
+      </c>
+      <c r="E263" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Jordon Ibe', appearances: 11 },</v>
+      </c>
+    </row>
+    <row r="264" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A264" t="s">
+        <v>229</v>
+      </c>
+      <c r="B264">
+        <v>2017</v>
+      </c>
+      <c r="C264">
+        <v>11</v>
+      </c>
+      <c r="D264">
+        <v>0</v>
+      </c>
+      <c r="E264" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Cheick Keita', appearances: 11 },</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A265" t="s">
+        <v>230</v>
+      </c>
+      <c r="B265">
+        <v>2006</v>
+      </c>
+      <c r="C265">
+        <v>11</v>
+      </c>
+      <c r="D265">
+        <v>1</v>
+      </c>
+      <c r="E265" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Chris Sutton', appearances: 11 },</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A266" t="s">
+        <v>334</v>
+      </c>
+      <c r="B266">
+        <v>2009</v>
+      </c>
+      <c r="C266">
+        <v>11</v>
+      </c>
+      <c r="D266">
+        <v>0</v>
+      </c>
+      <c r="E266" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Nigel Quashie', appearances: 11 },</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A267" t="s">
+        <v>231</v>
+      </c>
+      <c r="B267">
+        <v>2018</v>
+      </c>
+      <c r="C267">
+        <v>11</v>
+      </c>
+      <c r="D267">
+        <v>0</v>
+      </c>
+      <c r="E267" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Jason Lowe', appearances: 11 },</v>
+      </c>
+    </row>
+    <row r="268" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A268" t="s">
+        <v>335</v>
+      </c>
+      <c r="B268">
+        <v>2024</v>
+      </c>
+      <c r="C268">
+        <v>11</v>
+      </c>
+      <c r="D268">
+        <v>1</v>
+      </c>
+      <c r="E268" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Christoph Klarer', appearances: 11 },</v>
+      </c>
+    </row>
+    <row r="269" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A269" t="s">
+        <v>232</v>
+      </c>
+      <c r="B269">
+        <v>2006</v>
+      </c>
+      <c r="C269">
+        <v>11</v>
+      </c>
+      <c r="D269">
+        <v>0</v>
+      </c>
+      <c r="E269" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Marcos Painter', appearances: 11 },</v>
+      </c>
+    </row>
+    <row r="270" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A270" t="s">
+        <v>336</v>
+      </c>
+      <c r="B270">
+        <v>2012</v>
+      </c>
+      <c r="C270">
+        <v>10</v>
+      </c>
+      <c r="D270">
+        <v>3</v>
+      </c>
+      <c r="E270" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Leroy Lita', appearances: 10 },</v>
+      </c>
+    </row>
+    <row r="271" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A271" t="s">
+        <v>337</v>
+      </c>
+      <c r="B271">
+        <v>2016</v>
+      </c>
+      <c r="C271">
+        <v>10</v>
+      </c>
+      <c r="D271">
+        <v>1</v>
+      </c>
+      <c r="E271" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Will Buckley', appearances: 10 },</v>
+      </c>
+    </row>
+    <row r="272" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A272" t="s">
+        <v>338</v>
+      </c>
+      <c r="B272">
+        <v>2024</v>
+      </c>
+      <c r="C272">
+        <v>10</v>
+      </c>
+      <c r="D272">
+        <v>1</v>
+      </c>
+      <c r="E272" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Andre Dozzell', appearances: 10 },</v>
+      </c>
+    </row>
+    <row r="273" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A273" t="s">
+        <v>339</v>
+      </c>
+      <c r="B273">
+        <v>2022</v>
+      </c>
+      <c r="C273">
+        <v>10</v>
+      </c>
+      <c r="D273">
+        <v>0</v>
+      </c>
+      <c r="E273" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Teden Mengi', appearances: 10 },</v>
+      </c>
+    </row>
+    <row r="274" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A274" t="s">
+        <v>340</v>
+      </c>
+      <c r="B274">
+        <v>2024</v>
+      </c>
+      <c r="C274">
+        <v>10</v>
+      </c>
+      <c r="D274">
+        <v>2</v>
+      </c>
+      <c r="E274" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Willum Þór Willumsson', appearances: 10 },</v>
+      </c>
+    </row>
+    <row r="275" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A275" t="s">
+        <v>233</v>
+      </c>
+      <c r="B275">
+        <v>2020</v>
+      </c>
+      <c r="C275">
+        <v>10</v>
+      </c>
+      <c r="D275">
+        <v>0</v>
+      </c>
+      <c r="E275" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Josh McEachran', appearances: 10 },</v>
+      </c>
+    </row>
+    <row r="276" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A276" t="s">
+        <v>234</v>
+      </c>
+      <c r="B276">
+        <v>2013</v>
+      </c>
+      <c r="C276">
+        <v>10</v>
+      </c>
+      <c r="D276">
+        <v>1</v>
+      </c>
+      <c r="E276" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Darren Ambrose', appearances: 10 },</v>
+      </c>
+    </row>
+    <row r="277" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A277" t="s">
+        <v>341</v>
+      </c>
+      <c r="B277">
+        <v>2023</v>
+      </c>
+      <c r="C277">
+        <v>10</v>
+      </c>
+      <c r="D277">
+        <v>0</v>
+      </c>
+      <c r="E277" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Romelle Donovan', appearances: 10 },</v>
+      </c>
+    </row>
+    <row r="278" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A278" t="s">
+        <v>342</v>
+      </c>
+      <c r="B278">
+        <v>2024</v>
+      </c>
+      <c r="C278">
+        <v>10</v>
+      </c>
+      <c r="D278">
+        <v>0</v>
+      </c>
+      <c r="E278" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Marc Leonard', appearances: 10 },</v>
+      </c>
+    </row>
+    <row r="279" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A279" t="s">
+        <v>235</v>
+      </c>
+      <c r="B279">
+        <v>2024</v>
+      </c>
+      <c r="C279">
+        <v>9</v>
+      </c>
+      <c r="D279">
+        <v>0</v>
+      </c>
+      <c r="E279" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Alex Pritchard', appearances: 9 },</v>
+      </c>
+    </row>
+    <row r="280" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A280" t="s">
+        <v>236</v>
+      </c>
+      <c r="B280">
+        <v>2010</v>
+      </c>
+      <c r="C280">
+        <v>9</v>
+      </c>
+      <c r="D280">
+        <v>0</v>
+      </c>
+      <c r="E280" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Grégory Vignal', appearances: 9 },</v>
+      </c>
+    </row>
+    <row r="281" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A281" t="s">
+        <v>343</v>
+      </c>
+      <c r="B281">
+        <v>2000</v>
+      </c>
+      <c r="C281">
+        <v>9</v>
+      </c>
+      <c r="D281">
+        <v>0</v>
+      </c>
+      <c r="E281" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Thomas Myhre', appearances: 9 },</v>
+      </c>
+    </row>
+    <row r="282" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A282" t="s">
+        <v>344</v>
+      </c>
+      <c r="B282">
+        <v>2014</v>
+      </c>
+      <c r="C282">
+        <v>9</v>
+      </c>
+      <c r="D282">
+        <v>0</v>
+      </c>
+      <c r="E282" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Grant Hall', appearances: 9 },</v>
+      </c>
+    </row>
+    <row r="283" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A283" t="s">
+        <v>345</v>
+      </c>
+      <c r="B283">
+        <v>2018</v>
+      </c>
+      <c r="C283">
+        <v>9</v>
+      </c>
+      <c r="D283">
+        <v>0</v>
+      </c>
+      <c r="E283" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Carl Jenkinson', appearances: 9 },</v>
+      </c>
+    </row>
+    <row r="284" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A284" t="s">
+        <v>237</v>
+      </c>
+      <c r="B284">
+        <v>2020</v>
+      </c>
+      <c r="C284">
+        <v>9</v>
+      </c>
+      <c r="D284">
+        <v>0</v>
+      </c>
+      <c r="E284" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Caolan Boyd-Munce', appearances: 9 },</v>
+      </c>
+    </row>
+    <row r="285" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A285" t="s">
+        <v>346</v>
+      </c>
+      <c r="B285">
+        <v>2024</v>
+      </c>
+      <c r="C285">
+        <v>9</v>
+      </c>
+      <c r="D285">
+        <v>0</v>
+      </c>
+      <c r="E285" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Alfons Sampsted', appearances: 9 },</v>
+      </c>
+    </row>
+    <row r="286" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A286" t="s">
+        <v>347</v>
+      </c>
+      <c r="B286">
+        <v>2022</v>
+      </c>
+      <c r="C286">
+        <v>9</v>
+      </c>
+      <c r="D286">
+        <v>0</v>
+      </c>
+      <c r="E286" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Josh Williams', appearances: 9 },</v>
+      </c>
+    </row>
+    <row r="287" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A287" t="s">
+        <v>238</v>
+      </c>
+      <c r="B287">
+        <v>2000</v>
+      </c>
+      <c r="C287">
+        <v>9</v>
+      </c>
+      <c r="D287">
+        <v>0</v>
+      </c>
+      <c r="E287" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Eddie Newton', appearances: 9 },</v>
+      </c>
+    </row>
+    <row r="288" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A288" t="s">
+        <v>348</v>
+      </c>
+      <c r="B288">
+        <v>2009</v>
+      </c>
+      <c r="C288">
+        <v>8</v>
+      </c>
+      <c r="D288">
+        <v>0</v>
+      </c>
+      <c r="E288" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Carlos Costly', appearances: 8 },</v>
+      </c>
+    </row>
+    <row r="289" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A289" t="s">
+        <v>349</v>
+      </c>
+      <c r="B289">
+        <v>2014</v>
+      </c>
+      <c r="C289">
+        <v>8</v>
+      </c>
+      <c r="D289">
+        <v>0</v>
+      </c>
+      <c r="E289" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Tyler Blackett', appearances: 8 },</v>
+      </c>
+    </row>
+    <row r="290" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A290" t="s">
+        <v>239</v>
+      </c>
+      <c r="B290">
+        <v>2014</v>
+      </c>
+      <c r="C290">
+        <v>8</v>
+      </c>
+      <c r="D290">
+        <v>0</v>
+      </c>
+      <c r="E290" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Aaron Martin', appearances: 8 },</v>
+      </c>
+    </row>
+    <row r="291" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A291" t="s">
+        <v>350</v>
+      </c>
+      <c r="B291">
+        <v>2008</v>
+      </c>
+      <c r="C291">
+        <v>8</v>
+      </c>
+      <c r="D291">
+        <v>0</v>
+      </c>
+      <c r="E291" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Wilson Palacios', appearances: 8 },</v>
+      </c>
+    </row>
+    <row r="292" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A292" t="s">
+        <v>351</v>
+      </c>
+      <c r="B292">
+        <v>2024</v>
+      </c>
+      <c r="C292">
+        <v>8</v>
+      </c>
+      <c r="D292">
+        <v>0</v>
+      </c>
+      <c r="E292" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Taylor Gardner-Hickman', appearances: 8 },</v>
+      </c>
+    </row>
+    <row r="293" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A293" t="s">
+        <v>240</v>
+      </c>
+      <c r="B293">
+        <v>2015</v>
+      </c>
+      <c r="C293">
+        <v>8</v>
+      </c>
+      <c r="D293">
+        <v>0</v>
+      </c>
+      <c r="E293" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Nicolai Brock-Madsen', appearances: 8 },</v>
+      </c>
+    </row>
+    <row r="294" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A294" t="s">
+        <v>241</v>
+      </c>
+      <c r="B294">
+        <v>2020</v>
+      </c>
+      <c r="C294">
+        <v>8</v>
+      </c>
+      <c r="D294">
+        <v>1</v>
+      </c>
+      <c r="E294" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Odin Bailey', appearances: 8 },</v>
+      </c>
+    </row>
+    <row r="295" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A295" t="s">
+        <v>352</v>
+      </c>
+      <c r="B295">
+        <v>2018</v>
+      </c>
+      <c r="C295">
+        <v>8</v>
+      </c>
+      <c r="D295">
+        <v>0</v>
+      </c>
+      <c r="E295" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Cohen Bramall', appearances: 8 },</v>
+      </c>
+    </row>
+    <row r="296" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A296" t="s">
+        <v>242</v>
+      </c>
+      <c r="B296">
+        <v>2023</v>
+      </c>
+      <c r="C296">
+        <v>8</v>
+      </c>
+      <c r="D296">
+        <v>1</v>
+      </c>
+      <c r="E296" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Marcel Oakley', appearances: 8 },</v>
+      </c>
+    </row>
+    <row r="297" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A297" t="s">
+        <v>353</v>
+      </c>
+      <c r="B297">
+        <v>2013</v>
+      </c>
+      <c r="C297">
+        <v>7</v>
+      </c>
+      <c r="D297">
+        <v>0</v>
+      </c>
+      <c r="E297" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Aaron McLean', appearances: 7 },</v>
+      </c>
+    </row>
+    <row r="298" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A298" t="s">
+        <v>354</v>
+      </c>
+      <c r="B298">
+        <v>2021</v>
+      </c>
+      <c r="C298">
+        <v>7</v>
+      </c>
+      <c r="D298">
+        <v>0</v>
+      </c>
+      <c r="E298" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Yan Valery', appearances: 7 },</v>
+      </c>
+    </row>
+    <row r="299" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A299" t="s">
+        <v>355</v>
+      </c>
+      <c r="B299">
+        <v>2024</v>
+      </c>
+      <c r="C299">
+        <v>7</v>
+      </c>
+      <c r="D299">
+        <v>0</v>
+      </c>
+      <c r="E299" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Bailey Peacock-Farrell', appearances: 7 },</v>
+      </c>
+    </row>
+    <row r="300" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A300" t="s">
+        <v>356</v>
+      </c>
+      <c r="B300">
+        <v>2006</v>
+      </c>
+      <c r="C300">
+        <v>7</v>
+      </c>
+      <c r="D300">
+        <v>0</v>
+      </c>
+      <c r="E300" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Martin Latka', appearances: 7 },</v>
+      </c>
+    </row>
+    <row r="301" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A301" t="s">
+        <v>357</v>
+      </c>
+      <c r="B301">
+        <v>2014</v>
+      </c>
+      <c r="C301">
+        <v>7</v>
+      </c>
+      <c r="D301">
+        <v>2</v>
+      </c>
+      <c r="E301" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Scott Allan', appearances: 7 },</v>
+      </c>
+    </row>
+    <row r="302" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A302" t="s">
+        <v>243</v>
+      </c>
+      <c r="B302">
+        <v>2003</v>
+      </c>
+      <c r="C302">
+        <v>7</v>
+      </c>
+      <c r="D302">
+        <v>0</v>
+      </c>
+      <c r="E302" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Joey Hutchinson', appearances: 7 },</v>
+      </c>
+    </row>
+    <row r="303" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A303" t="s">
+        <v>244</v>
+      </c>
+      <c r="B303">
+        <v>2015</v>
+      </c>
+      <c r="C303">
+        <v>7</v>
+      </c>
+      <c r="D303">
+        <v>1</v>
+      </c>
+      <c r="E303" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Mark Duffy', appearances: 7 },</v>
+      </c>
+    </row>
+    <row r="304" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A304" t="s">
+        <v>358</v>
+      </c>
+      <c r="B304">
+        <v>2001</v>
+      </c>
+      <c r="C304">
+        <v>6</v>
+      </c>
+      <c r="D304">
+        <v>0</v>
+      </c>
+      <c r="E304" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Curtis Fleming', appearances: 6 },</v>
+      </c>
+    </row>
+    <row r="305" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A305" t="s">
+        <v>359</v>
+      </c>
+      <c r="B305">
+        <v>2001</v>
+      </c>
+      <c r="C305">
+        <v>6</v>
+      </c>
+      <c r="D305">
+        <v>0</v>
+      </c>
+      <c r="E305" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Alan Kelly', appearances: 6 },</v>
+      </c>
+    </row>
+    <row r="306" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A306" t="s">
+        <v>360</v>
+      </c>
+      <c r="B306">
+        <v>2010</v>
+      </c>
+      <c r="C306">
+        <v>6</v>
+      </c>
+      <c r="D306">
+        <v>0</v>
+      </c>
+      <c r="E306" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Teemu Tainio', appearances: 6 },</v>
+      </c>
+    </row>
+    <row r="307" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A307" t="s">
+        <v>361</v>
+      </c>
+      <c r="B307">
+        <v>2014</v>
+      </c>
+      <c r="C307">
+        <v>6</v>
+      </c>
+      <c r="D307">
+        <v>0</v>
+      </c>
+      <c r="E307" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Tom Thorpe', appearances: 6 },</v>
+      </c>
+    </row>
+    <row r="308" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A308" t="s">
+        <v>362</v>
+      </c>
+      <c r="B308">
+        <v>2014</v>
+      </c>
+      <c r="C308">
+        <v>6</v>
+      </c>
+      <c r="D308">
+        <v>0</v>
+      </c>
+      <c r="E308" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Brek Shea', appearances: 6 },</v>
+      </c>
+    </row>
+    <row r="309" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A309" t="s">
+        <v>363</v>
+      </c>
+      <c r="B309">
+        <v>2016</v>
+      </c>
+      <c r="C309">
+        <v>6</v>
+      </c>
+      <c r="D309">
+        <v>1</v>
+      </c>
+      <c r="E309" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Kyle Lafferty', appearances: 6 },</v>
+      </c>
+    </row>
+    <row r="310" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A310" t="s">
+        <v>364</v>
+      </c>
+      <c r="B310">
+        <v>2022</v>
+      </c>
+      <c r="C310">
+        <v>6</v>
+      </c>
+      <c r="D310">
+        <v>0</v>
+      </c>
+      <c r="E310" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Taylor Richards', appearances: 6 },</v>
+      </c>
+    </row>
+    <row r="311" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A311" t="s">
+        <v>365</v>
+      </c>
+      <c r="B311">
+        <v>2024</v>
+      </c>
+      <c r="C311">
+        <v>6</v>
+      </c>
+      <c r="D311">
+        <v>0</v>
+      </c>
+      <c r="E311" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Lyndon Dykes', appearances: 6 },</v>
+      </c>
+    </row>
+    <row r="312" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A312" t="s">
+        <v>366</v>
+      </c>
+      <c r="B312">
+        <v>2024</v>
+      </c>
+      <c r="C312">
+        <v>6</v>
+      </c>
+      <c r="D312">
+        <v>2</v>
+      </c>
+      <c r="E312" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Tomoki Iwata', appearances: 6 },</v>
+      </c>
+    </row>
+    <row r="313" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A313" t="s">
+        <v>367</v>
+      </c>
+      <c r="B313">
+        <v>2024</v>
+      </c>
+      <c r="C313">
+        <v>6</v>
+      </c>
+      <c r="D313">
+        <v>1</v>
+      </c>
+      <c r="E313" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Scott Wright', appearances: 6 },</v>
+      </c>
+    </row>
+    <row r="314" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A314" t="s">
+        <v>368</v>
+      </c>
+      <c r="B314">
+        <v>2011</v>
+      </c>
+      <c r="C314">
+        <v>6</v>
+      </c>
+      <c r="D314">
+        <v>2</v>
+      </c>
+      <c r="E314" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Obafemi Martins', appearances: 6 },</v>
+      </c>
+    </row>
+    <row r="315" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A315" t="s">
+        <v>369</v>
+      </c>
+      <c r="B315">
+        <v>2023</v>
+      </c>
+      <c r="C315">
+        <v>6</v>
+      </c>
+      <c r="D315">
+        <v>1</v>
+      </c>
+      <c r="E315" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Brandon Khela', appearances: 6 },</v>
+      </c>
+    </row>
+    <row r="316" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A316" t="s">
+        <v>370</v>
+      </c>
+      <c r="B316">
+        <v>2001</v>
+      </c>
+      <c r="C316">
+        <v>5</v>
+      </c>
+      <c r="D316">
+        <v>0</v>
+      </c>
+      <c r="E316" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Jamie Pollock', appearances: 5 },</v>
+      </c>
+    </row>
+    <row r="317" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A317" t="s">
+        <v>371</v>
+      </c>
+      <c r="B317">
+        <v>2007</v>
+      </c>
+      <c r="C317">
+        <v>5</v>
+      </c>
+      <c r="D317">
+        <v>1</v>
+      </c>
+      <c r="E317" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Andy Cole', appearances: 5 },</v>
+      </c>
+    </row>
+    <row r="318" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A318" t="s">
+        <v>245</v>
+      </c>
+      <c r="B318">
+        <v>2014</v>
+      </c>
+      <c r="C318">
+        <v>5</v>
+      </c>
+      <c r="D318">
+        <v>1</v>
+      </c>
+      <c r="E318" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Brian Howard', appearances: 5 },</v>
+      </c>
+    </row>
+    <row r="319" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A319" t="s">
+        <v>372</v>
+      </c>
+      <c r="B319">
+        <v>2017</v>
+      </c>
+      <c r="C319">
+        <v>5</v>
+      </c>
+      <c r="D319">
+        <v>0</v>
+      </c>
+      <c r="E319" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Jerome Sinclair', appearances: 5 },</v>
+      </c>
+    </row>
+    <row r="320" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A320" t="s">
+        <v>246</v>
+      </c>
+      <c r="B320">
+        <v>2021</v>
+      </c>
+      <c r="C320">
+        <v>5</v>
+      </c>
+      <c r="D320">
+        <v>0</v>
+      </c>
+      <c r="E320" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Amari Miller', appearances: 5 },</v>
+      </c>
+    </row>
+    <row r="321" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A321" t="s">
+        <v>373</v>
+      </c>
+      <c r="B321">
+        <v>2022</v>
+      </c>
+      <c r="C321">
+        <v>5</v>
+      </c>
+      <c r="D321">
+        <v>1</v>
+      </c>
+      <c r="E321" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Przemysław Płacheta', appearances: 5 },</v>
+      </c>
+    </row>
+    <row r="322" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A322" t="s">
+        <v>374</v>
+      </c>
+      <c r="B322">
+        <v>2002</v>
+      </c>
+      <c r="C322">
+        <v>5</v>
+      </c>
+      <c r="D322">
+        <v>0</v>
+      </c>
+      <c r="E322" t="str">
+        <f t="shared" si="4"/>
+        <v>{ name: 'Arkadiusz Bąk', appearances: 5 },</v>
+      </c>
+    </row>
+    <row r="323" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A323" t="s">
+        <v>247</v>
+      </c>
+      <c r="B323">
+        <v>2017</v>
+      </c>
+      <c r="C323">
+        <v>5</v>
+      </c>
+      <c r="D323">
+        <v>0</v>
+      </c>
+      <c r="E323" t="str">
+        <f t="shared" ref="E323:E386" si="5">"{ name: '" &amp; A323 &amp; "', appearances: " &amp; C323 &amp; " },"</f>
+        <v>{ name: 'Jack Storer', appearances: 5 },</v>
+      </c>
+    </row>
+    <row r="324" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A324" t="s">
+        <v>248</v>
+      </c>
+      <c r="B324">
+        <v>2018</v>
+      </c>
+      <c r="C324">
+        <v>5</v>
+      </c>
+      <c r="D324">
+        <v>0</v>
+      </c>
+      <c r="E324" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Bez Lubala', appearances: 5 },</v>
+      </c>
+    </row>
+    <row r="325" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A325" t="s">
+        <v>375</v>
+      </c>
+      <c r="B325">
+        <v>2024</v>
+      </c>
+      <c r="C325">
+        <v>5</v>
+      </c>
+      <c r="D325">
+        <v>1</v>
+      </c>
+      <c r="E325" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Luke Harris', appearances: 5 },</v>
+      </c>
+    </row>
+    <row r="326" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A326" t="s">
+        <v>376</v>
+      </c>
+      <c r="B326">
+        <v>2022</v>
+      </c>
+      <c r="C326">
+        <v>5</v>
+      </c>
+      <c r="D326">
+        <v>0</v>
+      </c>
+      <c r="E326" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Juan Castillo', appearances: 5 },</v>
+      </c>
+    </row>
+    <row r="327" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A327" t="s">
+        <v>377</v>
+      </c>
+      <c r="B327">
+        <v>2024</v>
+      </c>
+      <c r="C327">
+        <v>5</v>
+      </c>
+      <c r="D327">
+        <v>0</v>
+      </c>
+      <c r="E327" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Ayumu Yokoyama', appearances: 5 },</v>
+      </c>
+    </row>
+    <row r="328" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A328" t="s">
+        <v>249</v>
+      </c>
+      <c r="B328">
+        <v>2013</v>
+      </c>
+      <c r="C328">
+        <v>5</v>
+      </c>
+      <c r="D328">
+        <v>0</v>
+      </c>
+      <c r="E328" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Jake Jervis', appearances: 5 },</v>
+      </c>
+    </row>
+    <row r="329" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A329" t="s">
+        <v>378</v>
+      </c>
+      <c r="B329">
+        <v>2024</v>
+      </c>
+      <c r="C329">
+        <v>5</v>
+      </c>
+      <c r="D329">
+        <v>0</v>
+      </c>
+      <c r="E329" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Ryan Allsop', appearances: 5 },</v>
+      </c>
+    </row>
+    <row r="330" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A330" t="s">
+        <v>379</v>
+      </c>
+      <c r="B330">
+        <v>2001</v>
+      </c>
+      <c r="C330">
+        <v>4</v>
+      </c>
+      <c r="D330">
+        <v>0</v>
+      </c>
+      <c r="E330" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Carlos Ferrari', appearances: 4 },</v>
+      </c>
+    </row>
+    <row r="331" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A331" t="s">
+        <v>250</v>
+      </c>
+      <c r="B331">
+        <v>2002</v>
+      </c>
+      <c r="C331">
+        <v>4</v>
+      </c>
+      <c r="D331">
+        <v>0</v>
+      </c>
+      <c r="E331" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Tom Williams', appearances: 4 },</v>
+      </c>
+    </row>
+    <row r="332" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A332" t="s">
+        <v>251</v>
+      </c>
+      <c r="B332">
+        <v>2022</v>
+      </c>
+      <c r="C332">
+        <v>4</v>
+      </c>
+      <c r="D332">
+        <v>0</v>
+      </c>
+      <c r="E332" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Zach Jeacock', appearances: 4 },</v>
+      </c>
+    </row>
+    <row r="333" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A333" t="s">
+        <v>252</v>
+      </c>
+      <c r="B333">
+        <v>2020</v>
+      </c>
+      <c r="C333">
+        <v>4</v>
+      </c>
+      <c r="D333">
+        <v>0</v>
+      </c>
+      <c r="E333" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Jayden Reid', appearances: 4 },</v>
+      </c>
+    </row>
+    <row r="334" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A334" t="s">
+        <v>253</v>
+      </c>
+      <c r="B334">
+        <v>2000</v>
+      </c>
+      <c r="C334">
+        <v>4</v>
+      </c>
+      <c r="D334">
+        <v>0</v>
+      </c>
+      <c r="E334" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Jacques Williams', appearances: 4 },</v>
+      </c>
+    </row>
+    <row r="335" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A335" t="s">
+        <v>380</v>
+      </c>
+      <c r="B335">
+        <v>2001</v>
+      </c>
+      <c r="C335">
+        <v>4</v>
+      </c>
+      <c r="D335">
+        <v>0</v>
+      </c>
+      <c r="E335" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Steve Jenkins', appearances: 4 },</v>
+      </c>
+    </row>
+    <row r="336" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A336" t="s">
+        <v>381</v>
+      </c>
+      <c r="B336">
+        <v>2014</v>
+      </c>
+      <c r="C336">
+        <v>4</v>
+      </c>
+      <c r="D336">
+        <v>0</v>
+      </c>
+      <c r="E336" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Albert Rusnák', appearances: 4 },</v>
+      </c>
+    </row>
+    <row r="337" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A337" t="s">
+        <v>254</v>
+      </c>
+      <c r="B337">
+        <v>2022</v>
+      </c>
+      <c r="C337">
+        <v>4</v>
+      </c>
+      <c r="D337">
+        <v>0</v>
+      </c>
+      <c r="E337" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Ryan Stirk', appearances: 4 },</v>
+      </c>
+    </row>
+    <row r="338" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A338" t="s">
+        <v>382</v>
+      </c>
+      <c r="B338">
+        <v>2024</v>
+      </c>
+      <c r="C338">
+        <v>4</v>
+      </c>
+      <c r="D338">
+        <v>0</v>
+      </c>
+      <c r="E338" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Ben Davies', appearances: 4 },</v>
+      </c>
+    </row>
+    <row r="339" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A339" t="s">
+        <v>255</v>
+      </c>
+      <c r="B339">
+        <v>2003</v>
+      </c>
+      <c r="C339">
+        <v>4</v>
+      </c>
+      <c r="D339">
+        <v>0</v>
+      </c>
+      <c r="E339" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Craig Fagan', appearances: 4 },</v>
+      </c>
+    </row>
+    <row r="340" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A340" t="s">
+        <v>256</v>
+      </c>
+      <c r="B340">
+        <v>2022</v>
+      </c>
+      <c r="C340">
+        <v>4</v>
+      </c>
+      <c r="D340">
+        <v>0</v>
+      </c>
+      <c r="E340" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Tate Campbell', appearances: 4 },</v>
+      </c>
+    </row>
+    <row r="341" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A341" t="s">
+        <v>383</v>
+      </c>
+      <c r="B341">
+        <v>2000</v>
+      </c>
+      <c r="C341">
+        <v>3</v>
+      </c>
+      <c r="D341">
+        <v>0</v>
+      </c>
+      <c r="E341" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Richard Edghill', appearances: 3 },</v>
+      </c>
+    </row>
+    <row r="342" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A342" t="s">
+        <v>384</v>
+      </c>
+      <c r="B342">
+        <v>2000</v>
+      </c>
+      <c r="C342">
+        <v>3</v>
+      </c>
+      <c r="D342">
+        <v>0</v>
+      </c>
+      <c r="E342" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Gary Charles', appearances: 3 },</v>
+      </c>
+    </row>
+    <row r="343" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A343" t="s">
+        <v>385</v>
+      </c>
+      <c r="B343">
+        <v>2001</v>
+      </c>
+      <c r="C343">
+        <v>3</v>
+      </c>
+      <c r="D343">
+        <v>0</v>
+      </c>
+      <c r="E343" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Bjørn Otto Bragstad', appearances: 3 },</v>
+      </c>
+    </row>
+    <row r="344" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A344" t="s">
+        <v>386</v>
+      </c>
+      <c r="B344">
+        <v>2002</v>
+      </c>
+      <c r="C344">
+        <v>3</v>
+      </c>
+      <c r="D344">
+        <v>0</v>
+      </c>
+      <c r="E344" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Michael Hughes', appearances: 3 },</v>
+      </c>
+    </row>
+    <row r="345" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A345" t="s">
+        <v>387</v>
+      </c>
+      <c r="B345">
+        <v>2009</v>
+      </c>
+      <c r="C345">
+        <v>3</v>
+      </c>
+      <c r="D345">
+        <v>0</v>
+      </c>
+      <c r="E345" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Djimi Traoré', appearances: 3 },</v>
+      </c>
+    </row>
+    <row r="346" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A346" t="s">
+        <v>388</v>
+      </c>
+      <c r="B346">
+        <v>2012</v>
+      </c>
+      <c r="C346">
+        <v>3</v>
+      </c>
+      <c r="D346">
+        <v>0</v>
+      </c>
+      <c r="E346" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'James Hurst', appearances: 3 },</v>
+      </c>
+    </row>
+    <row r="347" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A347" t="s">
+        <v>389</v>
+      </c>
+      <c r="B347">
+        <v>2016</v>
+      </c>
+      <c r="C347">
+        <v>3</v>
+      </c>
+      <c r="D347">
+        <v>0</v>
+      </c>
+      <c r="E347" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Greg Halford', appearances: 3 },</v>
+      </c>
+    </row>
+    <row r="348" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A348" t="s">
+        <v>390</v>
+      </c>
+      <c r="B348">
+        <v>2017</v>
+      </c>
+      <c r="C348">
+        <v>3</v>
+      </c>
+      <c r="D348">
+        <v>0</v>
+      </c>
+      <c r="E348" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Liam Walsh', appearances: 3 },</v>
+      </c>
+    </row>
+    <row r="349" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A349" t="s">
+        <v>257</v>
+      </c>
+      <c r="B349">
+        <v>2015</v>
+      </c>
+      <c r="C349">
+        <v>3</v>
+      </c>
+      <c r="D349">
+        <v>0</v>
+      </c>
+      <c r="E349" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Guy Moussi', appearances: 3 },</v>
+      </c>
+    </row>
+    <row r="350" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A350" t="s">
+        <v>258</v>
+      </c>
+      <c r="B350">
+        <v>2016</v>
+      </c>
+      <c r="C350">
+        <v>3</v>
+      </c>
+      <c r="D350">
+        <v>0</v>
+      </c>
+      <c r="E350" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Charlee Adams', appearances: 3 },</v>
+      </c>
+    </row>
+    <row r="351" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A351" t="s">
+        <v>259</v>
+      </c>
+      <c r="B351">
+        <v>2019</v>
+      </c>
+      <c r="C351">
+        <v>3</v>
+      </c>
+      <c r="D351">
+        <v>0</v>
+      </c>
+      <c r="E351" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Geraldo Bajrami', appearances: 3 },</v>
+      </c>
+    </row>
+    <row r="352" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A352" t="s">
+        <v>260</v>
+      </c>
+      <c r="B352">
+        <v>2006</v>
+      </c>
+      <c r="C352">
+        <v>3</v>
+      </c>
+      <c r="D352">
+        <v>0</v>
+      </c>
+      <c r="E352" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Mathew Birley', appearances: 3 },</v>
+      </c>
+    </row>
+    <row r="353" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A353" t="s">
+        <v>261</v>
+      </c>
+      <c r="B353">
+        <v>2007</v>
+      </c>
+      <c r="C353">
+        <v>3</v>
+      </c>
+      <c r="D353">
+        <v>0</v>
+      </c>
+      <c r="E353" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Richard Kingson', appearances: 3 },</v>
+      </c>
+    </row>
+    <row r="354" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A354" t="s">
+        <v>262</v>
+      </c>
+      <c r="B354">
+        <v>2009</v>
+      </c>
+      <c r="C354">
+        <v>3</v>
+      </c>
+      <c r="D354">
+        <v>0</v>
+      </c>
+      <c r="E354" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Jay O'Shea', appearances: 3 },</v>
+      </c>
+    </row>
+    <row r="355" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A355" t="s">
+        <v>391</v>
+      </c>
+      <c r="B355">
+        <v>2000</v>
+      </c>
+      <c r="C355">
+        <v>2</v>
+      </c>
+      <c r="D355">
+        <v>0</v>
+      </c>
+      <c r="E355" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Michael Carrick', appearances: 2 },</v>
+      </c>
+    </row>
+    <row r="356" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A356" t="s">
+        <v>392</v>
+      </c>
+      <c r="B356">
+        <v>2000</v>
+      </c>
+      <c r="C356">
+        <v>2</v>
+      </c>
+      <c r="D356">
+        <v>0</v>
+      </c>
+      <c r="E356" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Stuart Campbell', appearances: 2 },</v>
+      </c>
+    </row>
+    <row r="357" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A357" t="s">
+        <v>393</v>
+      </c>
+      <c r="B357">
+        <v>2005</v>
+      </c>
+      <c r="C357">
+        <v>2</v>
+      </c>
+      <c r="D357">
+        <v>0</v>
+      </c>
+      <c r="E357" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Salif Diao', appearances: 2 },</v>
+      </c>
+    </row>
+    <row r="358" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A358" t="s">
+        <v>394</v>
+      </c>
+      <c r="B358">
+        <v>2007</v>
+      </c>
+      <c r="C358">
+        <v>2</v>
+      </c>
+      <c r="D358">
+        <v>0</v>
+      </c>
+      <c r="E358" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Borja Oubiña', appearances: 2 },</v>
+      </c>
+    </row>
+    <row r="359" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A359" t="s">
+        <v>263</v>
+      </c>
+      <c r="B359">
+        <v>2012</v>
+      </c>
+      <c r="C359">
+        <v>2</v>
+      </c>
+      <c r="D359">
+        <v>1</v>
+      </c>
+      <c r="E359" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Papa Bouba Diop', appearances: 2 },</v>
+      </c>
+    </row>
+    <row r="360" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A360" t="s">
+        <v>264</v>
+      </c>
+      <c r="B360">
+        <v>2013</v>
+      </c>
+      <c r="C360">
+        <v>2</v>
+      </c>
+      <c r="D360">
+        <v>0</v>
+      </c>
+      <c r="E360" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Dariusz Dudka', appearances: 2 },</v>
+      </c>
+    </row>
+    <row r="361" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A361" t="s">
+        <v>265</v>
+      </c>
+      <c r="B361">
+        <v>2014</v>
+      </c>
+      <c r="C361">
+        <v>2</v>
+      </c>
+      <c r="D361">
+        <v>0</v>
+      </c>
+      <c r="E361" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Denny Johnstone', appearances: 2 },</v>
+      </c>
+    </row>
+    <row r="362" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A362" t="s">
+        <v>395</v>
+      </c>
+      <c r="B362">
+        <v>2016</v>
+      </c>
+      <c r="C362">
+        <v>2</v>
+      </c>
+      <c r="D362">
+        <v>0</v>
+      </c>
+      <c r="E362" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Rhoys Wiggins', appearances: 2 },</v>
+      </c>
+    </row>
+    <row r="363" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A363" t="s">
+        <v>396</v>
+      </c>
+      <c r="B363">
+        <v>2003</v>
+      </c>
+      <c r="C363">
+        <v>2</v>
+      </c>
+      <c r="D363">
+        <v>0</v>
+      </c>
+      <c r="E363" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Ferdinand Coly', appearances: 2 },</v>
+      </c>
+    </row>
+    <row r="364" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A364" t="s">
+        <v>266</v>
+      </c>
+      <c r="B364">
+        <v>2003</v>
+      </c>
+      <c r="C364">
+        <v>2</v>
+      </c>
+      <c r="D364">
+        <v>0</v>
+      </c>
+      <c r="E364" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Luciano Figueroa', appearances: 2 },</v>
+      </c>
+    </row>
+    <row r="365" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A365" t="s">
+        <v>397</v>
+      </c>
+      <c r="B365">
+        <v>2012</v>
+      </c>
+      <c r="C365">
+        <v>2</v>
+      </c>
+      <c r="D365">
+        <v>0</v>
+      </c>
+      <c r="E365" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Ben Gordon', appearances: 2 },</v>
+      </c>
+    </row>
+    <row r="366" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A366" t="s">
+        <v>267</v>
+      </c>
+      <c r="B366">
+        <v>2016</v>
+      </c>
+      <c r="C366">
+        <v>2</v>
+      </c>
+      <c r="D366">
+        <v>0</v>
+      </c>
+      <c r="E366" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Shane Lowry', appearances: 2 },</v>
+      </c>
+    </row>
+    <row r="367" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A367" t="s">
+        <v>268</v>
+      </c>
+      <c r="B367">
+        <v>2019</v>
+      </c>
+      <c r="C367">
+        <v>2</v>
+      </c>
+      <c r="D367">
+        <v>0</v>
+      </c>
+      <c r="E367" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Agus Medina', appearances: 2 },</v>
+      </c>
+    </row>
+    <row r="368" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A368" t="s">
+        <v>269</v>
+      </c>
+      <c r="B368">
+        <v>2020</v>
+      </c>
+      <c r="C368">
+        <v>2</v>
+      </c>
+      <c r="D368">
+        <v>0</v>
+      </c>
+      <c r="E368" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Adan George', appearances: 2 },</v>
+      </c>
+    </row>
+    <row r="369" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A369" t="s">
+        <v>270</v>
+      </c>
+      <c r="B369">
+        <v>2021</v>
+      </c>
+      <c r="C369">
+        <v>2</v>
+      </c>
+      <c r="D369">
+        <v>0</v>
+      </c>
+      <c r="E369" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Keyendrah Simmonds', appearances: 2 },</v>
+      </c>
+    </row>
+    <row r="370" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A370" t="s">
+        <v>271</v>
+      </c>
+      <c r="B370">
+        <v>2021</v>
+      </c>
+      <c r="C370">
+        <v>2</v>
+      </c>
+      <c r="D370">
+        <v>0</v>
+      </c>
+      <c r="E370" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Mitch Roberts', appearances: 2 },</v>
+      </c>
+    </row>
+    <row r="371" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A371" t="s">
+        <v>272</v>
+      </c>
+      <c r="B371">
+        <v>2009</v>
+      </c>
+      <c r="C371">
+        <v>2</v>
+      </c>
+      <c r="D371">
+        <v>0</v>
+      </c>
+      <c r="E371" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Giovanny Espinoza', appearances: 2 },</v>
+      </c>
+    </row>
+    <row r="372" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A372" t="s">
+        <v>273</v>
+      </c>
+      <c r="B372">
+        <v>2010</v>
+      </c>
+      <c r="C372">
+        <v>2</v>
+      </c>
+      <c r="D372">
+        <v>0</v>
+      </c>
+      <c r="E372" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Enric Vallès', appearances: 2 },</v>
+      </c>
+    </row>
+    <row r="373" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A373" t="s">
+        <v>274</v>
+      </c>
+      <c r="B373">
+        <v>2021</v>
+      </c>
+      <c r="C373">
+        <v>2</v>
+      </c>
+      <c r="D373">
+        <v>0</v>
+      </c>
+      <c r="E373" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Andrés Prieto', appearances: 2 },</v>
+      </c>
+    </row>
+    <row r="374" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A374" t="s">
+        <v>398</v>
+      </c>
+      <c r="B374">
+        <v>2001</v>
+      </c>
+      <c r="C374">
+        <v>1</v>
+      </c>
+      <c r="D374">
+        <v>0</v>
+      </c>
+      <c r="E374" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Carl Tiler', appearances: 1 },</v>
+      </c>
+    </row>
+    <row r="375" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A375" t="s">
+        <v>275</v>
+      </c>
+      <c r="B375">
+        <v>2003</v>
+      </c>
+      <c r="C375">
+        <v>1</v>
+      </c>
+      <c r="D375">
+        <v>0</v>
+      </c>
+      <c r="E375" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Andy Marriott', appearances: 1 },</v>
+      </c>
+    </row>
+    <row r="376" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A376" t="s">
+        <v>399</v>
+      </c>
+      <c r="B376">
+        <v>2003</v>
+      </c>
+      <c r="C376">
+        <v>1</v>
+      </c>
+      <c r="D376">
+        <v>0</v>
+      </c>
+      <c r="E376" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Piotr Świerczewski', appearances: 1 },</v>
+      </c>
+    </row>
+    <row r="377" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A377" t="s">
+        <v>276</v>
+      </c>
+      <c r="B377">
+        <v>2004</v>
+      </c>
+      <c r="C377">
+        <v>1</v>
+      </c>
+      <c r="D377">
+        <v>0</v>
+      </c>
+      <c r="E377" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Andrew Barrowman', appearances: 1 },</v>
+      </c>
+    </row>
+    <row r="378" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A378" t="s">
+        <v>277</v>
+      </c>
+      <c r="B378">
+        <v>2008</v>
+      </c>
+      <c r="C378">
+        <v>1</v>
+      </c>
+      <c r="D378">
+        <v>0</v>
+      </c>
+      <c r="E378" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Jared Wilson', appearances: 1 },</v>
+      </c>
+    </row>
+    <row r="379" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A379" t="s">
+        <v>278</v>
+      </c>
+      <c r="B379">
+        <v>2009</v>
+      </c>
+      <c r="C379">
+        <v>1</v>
+      </c>
+      <c r="D379">
+        <v>0</v>
+      </c>
+      <c r="E379" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Ulises de la Cruz', appearances: 1 },</v>
+      </c>
+    </row>
+    <row r="380" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A380" t="s">
+        <v>279</v>
+      </c>
+      <c r="B380">
+        <v>2014</v>
+      </c>
+      <c r="C380">
+        <v>1</v>
+      </c>
+      <c r="D380">
+        <v>0</v>
+      </c>
+      <c r="E380" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Amari'i Bell', appearances: 1 },</v>
+      </c>
+    </row>
+    <row r="381" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A381" t="s">
+        <v>280</v>
+      </c>
+      <c r="B381">
+        <v>2016</v>
+      </c>
+      <c r="C381">
+        <v>1</v>
+      </c>
+      <c r="D381">
+        <v>0</v>
+      </c>
+      <c r="E381" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Corey O'Keeffe', appearances: 1 },</v>
+      </c>
+    </row>
+    <row r="382" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A382" t="s">
+        <v>281</v>
+      </c>
+      <c r="B382">
+        <v>2020</v>
+      </c>
+      <c r="C382">
+        <v>1</v>
+      </c>
+      <c r="D382">
+        <v>0</v>
+      </c>
+      <c r="E382" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Ryan Burke', appearances: 1 },</v>
+      </c>
+    </row>
+    <row r="383" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A383" t="s">
+        <v>282</v>
+      </c>
+      <c r="B383">
+        <v>2020</v>
+      </c>
+      <c r="C383">
+        <v>1</v>
+      </c>
+      <c r="D383">
+        <v>0</v>
+      </c>
+      <c r="E383" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Miguel Fernández', appearances: 1 },</v>
+      </c>
+    </row>
+    <row r="384" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A384" t="s">
+        <v>283</v>
+      </c>
+      <c r="B384">
+        <v>2005</v>
+      </c>
+      <c r="C384">
+        <v>1</v>
+      </c>
+      <c r="D384">
+        <v>0</v>
+      </c>
+      <c r="E384" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Peter Till', appearances: 1 },</v>
+      </c>
+    </row>
+    <row r="385" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A385" t="s">
+        <v>284</v>
+      </c>
+      <c r="B385">
+        <v>2006</v>
+      </c>
+      <c r="C385">
+        <v>1</v>
+      </c>
+      <c r="D385">
+        <v>0</v>
+      </c>
+      <c r="E385" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Sam Oji', appearances: 1 },</v>
+      </c>
+    </row>
+    <row r="386" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A386" t="s">
+        <v>285</v>
+      </c>
+      <c r="B386">
+        <v>2007</v>
+      </c>
+      <c r="C386">
+        <v>1</v>
+      </c>
+      <c r="D386">
+        <v>0</v>
+      </c>
+      <c r="E386" t="str">
+        <f t="shared" si="5"/>
+        <v>{ name: 'Sone Aluko', appearances: 1 },</v>
+      </c>
+    </row>
+    <row r="387" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A387" t="s">
+        <v>286</v>
+      </c>
+      <c r="B387">
+        <v>2009</v>
+      </c>
+      <c r="C387">
+        <v>1</v>
+      </c>
+      <c r="D387">
+        <v>0</v>
+      </c>
+      <c r="E387" t="str">
+        <f t="shared" ref="E387:E396" si="6">"{ name: '" &amp; A387 &amp; "', appearances: " &amp; C387 &amp; " },"</f>
+        <v>{ name: 'Robin Shroot', appearances: 1 },</v>
+      </c>
+    </row>
+    <row r="388" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A388" t="s">
+        <v>287</v>
+      </c>
+      <c r="B388">
+        <v>2009</v>
+      </c>
+      <c r="C388">
+        <v>1</v>
+      </c>
+      <c r="D388">
+        <v>0</v>
+      </c>
+      <c r="E388" t="str">
+        <f t="shared" si="6"/>
+        <v>{ name: 'Dan Preston', appearances: 1 },</v>
+      </c>
+    </row>
+    <row r="389" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A389" t="s">
+        <v>288</v>
+      </c>
+      <c r="B389">
+        <v>2009</v>
+      </c>
+      <c r="C389">
+        <v>1</v>
+      </c>
+      <c r="D389">
+        <v>0</v>
+      </c>
+      <c r="E389" t="str">
+        <f t="shared" si="6"/>
+        <v>{ name: 'Ashley Sammons', appearances: 1 },</v>
+      </c>
+    </row>
+    <row r="390" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A390" t="s">
+        <v>289</v>
+      </c>
+      <c r="B390">
+        <v>2011</v>
+      </c>
+      <c r="C390">
+        <v>1</v>
+      </c>
+      <c r="D390">
+        <v>0</v>
+      </c>
+      <c r="E390" t="str">
+        <f t="shared" si="6"/>
+        <v>{ name: 'Akwasi Asante', appearances: 1 },</v>
+      </c>
+    </row>
+    <row r="391" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A391" t="s">
+        <v>290</v>
+      </c>
+      <c r="B391">
+        <v>2012</v>
+      </c>
+      <c r="C391">
+        <v>1</v>
+      </c>
+      <c r="D391">
+        <v>0</v>
+      </c>
+      <c r="E391" t="str">
+        <f t="shared" si="6"/>
+        <v>{ name: 'Eddy Gnahoré', appearances: 1 },</v>
+      </c>
+    </row>
+    <row r="392" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A392" t="s">
+        <v>291</v>
+      </c>
+      <c r="B392">
+        <v>2012</v>
+      </c>
+      <c r="C392">
+        <v>1</v>
+      </c>
+      <c r="D392">
+        <v>0</v>
+      </c>
+      <c r="E392" t="str">
+        <f t="shared" si="6"/>
+        <v>{ name: 'David Lucas', appearances: 1 },</v>
+      </c>
+    </row>
+    <row r="393" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A393" t="s">
+        <v>292</v>
+      </c>
+      <c r="B393">
+        <v>2013</v>
+      </c>
+      <c r="C393">
+        <v>1</v>
+      </c>
+      <c r="D393">
+        <v>0</v>
+      </c>
+      <c r="E393" t="str">
+        <f t="shared" si="6"/>
+        <v>{ name: 'Reece Hales', appearances: 1 },</v>
+      </c>
+    </row>
+    <row r="394" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A394" t="s">
+        <v>293</v>
+      </c>
+      <c r="B394">
+        <v>2014</v>
+      </c>
+      <c r="C394">
+        <v>1</v>
+      </c>
+      <c r="D394">
+        <v>0</v>
+      </c>
+      <c r="E394" t="str">
+        <f t="shared" si="6"/>
+        <v>{ name: 'Gavin Gunning', appearances: 1 },</v>
+      </c>
+    </row>
+    <row r="395" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A395" t="s">
+        <v>294</v>
+      </c>
+      <c r="B395">
+        <v>2018</v>
+      </c>
+      <c r="C395">
+        <v>1</v>
+      </c>
+      <c r="D395">
+        <v>0</v>
+      </c>
+      <c r="E395" t="str">
+        <f t="shared" si="6"/>
+        <v>{ name: 'Dan Scarr', appearances: 1 },</v>
+      </c>
+    </row>
+    <row r="396" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A396" t="s">
+        <v>295</v>
+      </c>
+      <c r="B396">
+        <v>2020</v>
+      </c>
+      <c r="C396">
+        <v>1</v>
+      </c>
+      <c r="D396">
+        <v>0</v>
+      </c>
+      <c r="E396" t="str">
+        <f>"{ name: '" &amp; A396 &amp; "', appearances: " &amp; C396 &amp; " }"</f>
+        <v>{ name: 'Jack Concannon', appearances: 1 }</v>
       </c>
     </row>
   </sheetData>

</xml_diff>